<commit_message>
Idiot proof features added to Report method
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="31" count="31">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="34" count="34">
   <x:si>
     <x:t>az</x:t>
   </x:si>
@@ -43,79 +43,25 @@
     <x:t>patchpanelport</x:t>
   </x:si>
   <x:si>
-    <x:t>gru1</x:t>
+    <x:t>gru3</x:t>
   </x:si>
   <x:si>
     <x:t>gru</x:t>
   </x:si>
   <x:si>
-    <x:t>2</x:t>
-  </x:si>
-  <x:si>
-    <x:t>embratel</x:t>
-  </x:si>
-  <x:si>
-    <x:t>gru1-br-cor-r2</x:t>
+    <x:t>1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>google</x:t>
+  </x:si>
+  <x:si>
+    <x:t>gru3-br-cor-r2</x:t>
   </x:si>
   <x:si>
     <x:t>xe-1/0/0</x:t>
   </x:si>
   <x:si>
     <x:t>pp1</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1</x:t>
-  </x:si>
-  <x:si>
-    <x:t>akamai</x:t>
-  </x:si>
-  <x:si>
-    <x:t>3</x:t>
-  </x:si>
-  <x:si>
-    <x:t>telefonica</x:t>
-  </x:si>
-  <x:si>
-    <x:t>gru1-br-cor-r3</x:t>
-  </x:si>
-  <x:si>
-    <x:t>pp2</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1/2</x:t>
-  </x:si>
-  <x:si>
-    <x:t>4</x:t>
-  </x:si>
-  <x:si>
-    <x:t>gru1-br-cor-r4</x:t>
-  </x:si>
-  <x:si>
-    <x:t>et-0/0/11</x:t>
-  </x:si>
-  <x:si>
-    <x:t>3/4</x:t>
-  </x:si>
-  <x:si>
-    <x:t>5</x:t>
-  </x:si>
-  <x:si>
-    <x:t>microsoft</x:t>
-  </x:si>
-  <x:si>
-    <x:t>et-0/0/1</x:t>
-  </x:si>
-  <x:si>
-    <x:t>10</x:t>
-  </x:si>
-  <x:si>
-    <x:t>gru3</x:t>
-  </x:si>
-  <x:si>
-    <x:t>google</x:t>
-  </x:si>
-  <x:si>
-    <x:t>gru3-br-cor-r2</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -521,7 +467,7 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="E2" s="0" t="n">
-        <x:v>10</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="F2" s="0" t="s">
         <x:v>13</x:v>
@@ -534,151 +480,6 @@
       </x:c>
       <x:c r="I2" s="0" t="s">
         <x:v>11</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="3" spans="1:9">
-      <x:c r="A3" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="B3" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="C3" s="0" t="s">
-        <x:v>16</x:v>
-      </x:c>
-      <x:c r="D3" s="0" t="s">
-        <x:v>17</x:v>
-      </x:c>
-      <x:c r="E3" s="0" t="n">
-        <x:v>100</x:v>
-      </x:c>
-      <x:c r="F3" s="0" t="s">
-        <x:v>13</x:v>
-      </x:c>
-      <x:c r="G3" s="0" t="s">
-        <x:v>14</x:v>
-      </x:c>
-      <x:c r="H3" s="0" t="s">
-        <x:v>15</x:v>
-      </x:c>
-      <x:c r="I3" s="0" t="s">
-        <x:v>16</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="4" spans="1:9">
-      <x:c r="A4" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="B4" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="C4" s="0" t="s">
-        <x:v>18</x:v>
-      </x:c>
-      <x:c r="D4" s="0" t="s">
-        <x:v>19</x:v>
-      </x:c>
-      <x:c r="E4" s="0" t="n">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="F4" s="0" t="s">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="G4" s="0" t="s">
-        <x:v>14</x:v>
-      </x:c>
-      <x:c r="H4" s="0" t="s">
-        <x:v>21</x:v>
-      </x:c>
-      <x:c r="I4" s="0" t="s">
-        <x:v>22</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="5" spans="1:9">
-      <x:c r="A5" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="B5" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="C5" s="0" t="s">
-        <x:v>23</x:v>
-      </x:c>
-      <x:c r="D5" s="0" t="s">
-        <x:v>17</x:v>
-      </x:c>
-      <x:c r="E5" s="0" t="n">
-        <x:v>100</x:v>
-      </x:c>
-      <x:c r="F5" s="0" t="s">
-        <x:v>24</x:v>
-      </x:c>
-      <x:c r="G5" s="0" t="s">
-        <x:v>25</x:v>
-      </x:c>
-      <x:c r="H5" s="0" t="s">
-        <x:v>21</x:v>
-      </x:c>
-      <x:c r="I5" s="0" t="s">
-        <x:v>26</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="6" spans="1:9">
-      <x:c r="A6" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="B6" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="C6" s="0" t="s">
-        <x:v>27</x:v>
-      </x:c>
-      <x:c r="D6" s="0" t="s">
-        <x:v>28</x:v>
-      </x:c>
-      <x:c r="E6" s="0" t="n">
-        <x:v>100</x:v>
-      </x:c>
-      <x:c r="F6" s="0" t="s">
-        <x:v>24</x:v>
-      </x:c>
-      <x:c r="G6" s="0" t="s">
-        <x:v>29</x:v>
-      </x:c>
-      <x:c r="H6" s="0" t="s">
-        <x:v>21</x:v>
-      </x:c>
-      <x:c r="I6" s="0" t="s">
-        <x:v>30</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="7" spans="1:9">
-      <x:c r="A7" s="0" t="s">
-        <x:v>31</x:v>
-      </x:c>
-      <x:c r="B7" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="C7" s="0" t="s">
-        <x:v>16</x:v>
-      </x:c>
-      <x:c r="D7" s="0" t="s">
-        <x:v>32</x:v>
-      </x:c>
-      <x:c r="E7" s="0" t="n">
-        <x:v>100</x:v>
-      </x:c>
-      <x:c r="F7" s="0" t="s">
-        <x:v>33</x:v>
-      </x:c>
-      <x:c r="G7" s="0" t="s">
-        <x:v>14</x:v>
-      </x:c>
-      <x:c r="H7" s="0" t="s">
-        <x:v>15</x:v>
-      </x:c>
-      <x:c r="I7" s="0" t="s">
-        <x:v>16</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
Update method searching for a ID in a specific AZ
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="34" count="34">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="36" count="36">
   <x:si>
     <x:t>az</x:t>
   </x:si>
@@ -55,7 +55,7 @@
     <x:t>google</x:t>
   </x:si>
   <x:si>
-    <x:t>gru3-br-cor-r2</x:t>
+    <x:t>gru3-br-cor-r10</x:t>
   </x:si>
   <x:si>
     <x:t>xe-1/0/0</x:t>

</xml_diff>

<commit_message>
Issue on add patch-panel fixed.
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="36" count="36">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="23" count="23">
   <x:si>
     <x:t>az</x:t>
   </x:si>
@@ -43,85 +43,25 @@
     <x:t>patchpanelport</x:t>
   </x:si>
   <x:si>
-    <x:t>gru1</x:t>
-  </x:si>
-  <x:si>
-    <x:t>gru</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2</x:t>
-  </x:si>
-  <x:si>
-    <x:t>embratel</x:t>
-  </x:si>
-  <x:si>
-    <x:t>gru1-br-cor-r2</x:t>
-  </x:si>
-  <x:si>
-    <x:t>xe-1/0/0</x:t>
+    <x:t>iad55</x:t>
+  </x:si>
+  <x:si>
+    <x:t>iad</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>akamai</x:t>
+  </x:si>
+  <x:si>
+    <x:t>iad55-br-cor-r3</x:t>
+  </x:si>
+  <x:si>
+    <x:t>et-0/0/11</x:t>
   </x:si>
   <x:si>
     <x:t>pp1</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1</x:t>
-  </x:si>
-  <x:si>
-    <x:t>akamai</x:t>
-  </x:si>
-  <x:si>
-    <x:t>3</x:t>
-  </x:si>
-  <x:si>
-    <x:t>telefonica</x:t>
-  </x:si>
-  <x:si>
-    <x:t>gru1-br-cor-r3</x:t>
-  </x:si>
-  <x:si>
-    <x:t>pp2</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1/2</x:t>
-  </x:si>
-  <x:si>
-    <x:t>4</x:t>
-  </x:si>
-  <x:si>
-    <x:t>gru1-br-cor-r4</x:t>
-  </x:si>
-  <x:si>
-    <x:t>et-0/0/11</x:t>
-  </x:si>
-  <x:si>
-    <x:t>3/4</x:t>
-  </x:si>
-  <x:si>
-    <x:t>5</x:t>
-  </x:si>
-  <x:si>
-    <x:t>microsoft</x:t>
-  </x:si>
-  <x:si>
-    <x:t>et-0/0/1</x:t>
-  </x:si>
-  <x:si>
-    <x:t>10</x:t>
-  </x:si>
-  <x:si>
-    <x:t>gru3</x:t>
-  </x:si>
-  <x:si>
-    <x:t>google</x:t>
-  </x:si>
-  <x:si>
-    <x:t>gru3-br-cor-r10</x:t>
-  </x:si>
-  <x:si>
-    <x:t>26</x:t>
-  </x:si>
-  <x:si>
-    <x:t>xe-0/0/0</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -527,7 +467,7 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="E2" s="0" t="n">
-        <x:v>10</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="F2" s="0" t="s">
         <x:v>13</x:v>
@@ -539,180 +479,6 @@
         <x:v>15</x:v>
       </x:c>
       <x:c r="I2" s="0" t="s">
-        <x:v>11</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="3" spans="1:9">
-      <x:c r="A3" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="B3" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="C3" s="0" t="s">
-        <x:v>16</x:v>
-      </x:c>
-      <x:c r="D3" s="0" t="s">
-        <x:v>17</x:v>
-      </x:c>
-      <x:c r="E3" s="0" t="n">
-        <x:v>100</x:v>
-      </x:c>
-      <x:c r="F3" s="0" t="s">
-        <x:v>13</x:v>
-      </x:c>
-      <x:c r="G3" s="0" t="s">
-        <x:v>14</x:v>
-      </x:c>
-      <x:c r="H3" s="0" t="s">
-        <x:v>15</x:v>
-      </x:c>
-      <x:c r="I3" s="0" t="s">
-        <x:v>16</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="4" spans="1:9">
-      <x:c r="A4" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="B4" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="C4" s="0" t="s">
-        <x:v>18</x:v>
-      </x:c>
-      <x:c r="D4" s="0" t="s">
-        <x:v>19</x:v>
-      </x:c>
-      <x:c r="E4" s="0" t="n">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="F4" s="0" t="s">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="G4" s="0" t="s">
-        <x:v>14</x:v>
-      </x:c>
-      <x:c r="H4" s="0" t="s">
-        <x:v>21</x:v>
-      </x:c>
-      <x:c r="I4" s="0" t="s">
-        <x:v>22</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="5" spans="1:9">
-      <x:c r="A5" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="B5" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="C5" s="0" t="s">
-        <x:v>23</x:v>
-      </x:c>
-      <x:c r="D5" s="0" t="s">
-        <x:v>17</x:v>
-      </x:c>
-      <x:c r="E5" s="0" t="n">
-        <x:v>100</x:v>
-      </x:c>
-      <x:c r="F5" s="0" t="s">
-        <x:v>24</x:v>
-      </x:c>
-      <x:c r="G5" s="0" t="s">
-        <x:v>25</x:v>
-      </x:c>
-      <x:c r="H5" s="0" t="s">
-        <x:v>21</x:v>
-      </x:c>
-      <x:c r="I5" s="0" t="s">
-        <x:v>26</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="6" spans="1:9">
-      <x:c r="A6" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="B6" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="C6" s="0" t="s">
-        <x:v>27</x:v>
-      </x:c>
-      <x:c r="D6" s="0" t="s">
-        <x:v>28</x:v>
-      </x:c>
-      <x:c r="E6" s="0" t="n">
-        <x:v>100</x:v>
-      </x:c>
-      <x:c r="F6" s="0" t="s">
-        <x:v>24</x:v>
-      </x:c>
-      <x:c r="G6" s="0" t="s">
-        <x:v>29</x:v>
-      </x:c>
-      <x:c r="H6" s="0" t="s">
-        <x:v>21</x:v>
-      </x:c>
-      <x:c r="I6" s="0" t="s">
-        <x:v>30</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="7" spans="1:9">
-      <x:c r="A7" s="0" t="s">
-        <x:v>31</x:v>
-      </x:c>
-      <x:c r="B7" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="C7" s="0" t="s">
-        <x:v>16</x:v>
-      </x:c>
-      <x:c r="D7" s="0" t="s">
-        <x:v>32</x:v>
-      </x:c>
-      <x:c r="E7" s="0" t="n">
-        <x:v>100</x:v>
-      </x:c>
-      <x:c r="F7" s="0" t="s">
-        <x:v>33</x:v>
-      </x:c>
-      <x:c r="G7" s="0" t="s">
-        <x:v>14</x:v>
-      </x:c>
-      <x:c r="H7" s="0" t="s">
-        <x:v>15</x:v>
-      </x:c>
-      <x:c r="I7" s="0" t="s">
-        <x:v>16</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="8" spans="1:9">
-      <x:c r="A8" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="B8" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="C8" s="0" t="s">
-        <x:v>34</x:v>
-      </x:c>
-      <x:c r="D8" s="0" t="s">
-        <x:v>28</x:v>
-      </x:c>
-      <x:c r="E8" s="0" t="n">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="F8" s="0" t="s">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="G8" s="0" t="s">
-        <x:v>35</x:v>
-      </x:c>
-      <x:c r="H8" s="0" t="s">
-        <x:v>21</x:v>
-      </x:c>
-      <x:c r="I8" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
     </x:row>

</xml_diff>

<commit_message>
Download CSV button added to Seach page
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -43,25 +43,46 @@
     <x:t>patchpanelport</x:t>
   </x:si>
   <x:si>
-    <x:t>iad55</x:t>
-  </x:si>
-  <x:si>
-    <x:t>iad</x:t>
+    <x:t>gru1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>gru</x:t>
   </x:si>
   <x:si>
     <x:t>1</x:t>
   </x:si>
   <x:si>
-    <x:t>akamai</x:t>
-  </x:si>
-  <x:si>
-    <x:t>iad55-br-cor-r3</x:t>
+    <x:t>google</x:t>
+  </x:si>
+  <x:si>
+    <x:t>gru1-br-cor-r3</x:t>
   </x:si>
   <x:si>
     <x:t>et-0/0/11</x:t>
   </x:si>
   <x:si>
     <x:t>pp1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>microsoft</x:t>
+  </x:si>
+  <x:si>
+    <x:t>gru1-br-tra-r3</x:t>
+  </x:si>
+  <x:si>
+    <x:t>4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>globenet</x:t>
+  </x:si>
+  <x:si>
+    <x:t>gru1-br-cor-r4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>et-0/0/37</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -482,6 +503,64 @@
         <x:v>11</x:v>
       </x:c>
     </x:row>
+    <x:row r="3" spans="1:9">
+      <x:c r="A3" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="B3" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="C3" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="D3" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="E3" s="0" t="n">
+        <x:v>100</x:v>
+      </x:c>
+      <x:c r="F3" s="0" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="G3" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="H3" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="I3" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:9">
+      <x:c r="A4" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="B4" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="C4" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="D4" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="E4" s="0" t="n">
+        <x:v>100</x:v>
+      </x:c>
+      <x:c r="F4" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="G4" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="H4" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="I4" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>

</xml_diff>